<commit_message>
Set the default project to the the app project as it is supposed to be
</commit_message>
<xml_diff>
--- a/OfficeApp1/bin/Debug/Book1.xlsx
+++ b/OfficeApp1/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R8a652e1cf1074c3f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6ae588941515481f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{0ebba3ec-3a43-4c99-ad1b-41638fdec034}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{939fd62f-3965-42e0-877a-87abee254308}">
   <we:reference id="6ce2b5b0-9907-4cec-aa0a-d7e1266dca6c" version="1.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>